<commit_message>
arreglo css had y excel
</commit_message>
<xml_diff>
--- a/files/fundamentosSI.xlsx
+++ b/files/fundamentosSI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\html\angelicap12.github.io\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96FAC65D-B237-40BC-893D-98825838F0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6170D3AC-1D3D-4313-9B3F-4947C04D29EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{200D975C-C180-4C83-84B4-2AB07AE4474F}"/>
   </bookViews>
@@ -35,15 +35,73 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Puertos de entrada y salida</t>
+  </si>
+  <si>
+    <t>Socket del procesador</t>
+  </si>
+  <si>
+    <t>Ranura de expansión PCI-Express x16</t>
+  </si>
+  <si>
+    <t>Conector de energía</t>
+  </si>
+  <si>
+    <t>Conector SATA</t>
+  </si>
+  <si>
+    <t>Ranuras de expansión de memoria RAM</t>
+  </si>
+  <si>
+    <t>Conector IDE</t>
+  </si>
+  <si>
+    <t>Puente sur</t>
+  </si>
+  <si>
+    <t>Puente norte</t>
+  </si>
+  <si>
+    <t>Socket pila</t>
+  </si>
+  <si>
+    <t>Ranura PCI</t>
+  </si>
+  <si>
+    <t>BIOS</t>
+  </si>
+  <si>
+    <t>Conector FDD</t>
+  </si>
+  <si>
+    <t>Ranura de expansión PCI-Express x4</t>
+  </si>
+  <si>
+    <t>NOMBRES</t>
+  </si>
+  <si>
+    <t>Ingrese en el numero el nombre correspondiente</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF001A1E"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +120,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -83,6 +168,123 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>181408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B27BF8BD-2AF3-D3E4-CF25-C3055FAE252E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6657975" cy="3038908"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectángulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B37A44D-5B87-C73C-9C95-610156AAD8EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3943350" y="723900"/>
+          <a:ext cx="295275" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-CO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,12 +604,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18414CA1-6D84-4A0E-858C-62554FCA0A7D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="10" max="10" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>2</v>
+      </c>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3</v>
+      </c>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="5">
+        <v>4</v>
+      </c>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="5">
+        <v>5</v>
+      </c>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="5">
+        <v>6</v>
+      </c>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="5">
+        <v>7</v>
+      </c>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="5">
+        <v>8</v>
+      </c>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="5">
+        <v>9</v>
+      </c>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="5">
+        <v>10</v>
+      </c>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="5">
+        <v>11</v>
+      </c>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="5">
+        <v>12</v>
+      </c>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="5">
+        <v>13</v>
+      </c>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="5">
+        <v>14</v>
+      </c>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>